<commit_message>
Add TikTok comment extractor with engagement filtering
</commit_message>
<xml_diff>
--- a/excel_to_test/quán_ngon_quận_10_v2.xlsx
+++ b/excel_to_test/quán_ngon_quận_10_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chatbot\tiktok_cao_cmt\QUANAN\q10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chatbot\tiktok_cao_cmt\for_test2\excel_to_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>usn_time</t>
   </si>
@@ -45,12 +45,6 @@
     <t>https://www.tiktok.com/@thudidaurua/video/7329436793617829121</t>
   </si>
   <si>
-    <t>dianthoii__2024_17_03</t>
-  </si>
-  <si>
-    <t>https://www.tiktok.com/@dianthoii_/video/7347171148477500673</t>
-  </si>
-  <si>
     <t>thudidaurua_2024_22_07</t>
   </si>
   <si>
@@ -73,15 +67,6 @@
   </si>
   <si>
     <t>Buffet nướng/ lẩu</t>
-  </si>
-  <si>
-    <t>Món ngon ở Q5</t>
-  </si>
-  <si>
-    <t>Quận 5, TP. HCM</t>
-  </si>
-  <si>
-    <t>Nguoisaigon, quận 5</t>
   </si>
   <si>
     <t>Cửu Long Quán</t>
@@ -475,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,73 +503,56 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>